<commit_message>
feat: Implement Excel automation examples covering core spreadsheet operations
- Cell value manipulation and merging operations
- Row/column sizing, insertion, and freeze panes functionality
- Formula implementation and range operations
- Document properties and worksheet management
- Hidden sheet operations and cell styling with custom fonts/colors
- Modular architecture with centralized console interface and error handling
</commit_message>
<xml_diff>
--- a/Openize.OpenXML-SDK.Examples.Usage/Documents/Workbook/MultipleSheets.xlsx
+++ b/Openize.OpenXML-SDK.Examples.Usage/Documents/Workbook/MultipleSheets.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R4fd97a9333c74af6"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" r:id="Rd3abf1b303ea4950"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" r:id="R2135f50239ce4fd3"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Raf277387919d452c"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" r:id="R73d52a4c761a4b88"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" r:id="Ra428c69ad15140de"/>
   </x:sheets>
 </x:workbook>
 </file>

</xml_diff>